<commit_message>
fix: Don't allow multivalues for ancestry category
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.13.xlsx
+++ b/schema_definitions/template_schema_v1.13.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karatugo/Documents/GitHub/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE888E5-F8A4-CE46-A460-75B8B5F66551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0B5D89-46A1-8646-88B7-5317EE892896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4060" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5440" yWindow="-25660" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="233">
   <si>
     <t>NAME</t>
   </si>
@@ -3302,8 +3302,8 @@
   </sheetPr>
   <dimension ref="A1:R1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3701,12 +3701,10 @@
       <c r="N9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="O9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2"/>
       <c r="Q9" s="2" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
fix: Revert disallow multiple ancestry category
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.13.xlsx
+++ b/schema_definitions/template_schema_v1.13.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karatugo/Documents/GitHub/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0B5D89-46A1-8646-88B7-5317EE892896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDCD825-431E-8549-8382-DA4664EBB6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5440" yWindow="-25660" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="233">
   <si>
     <t>NAME</t>
   </si>
@@ -3303,7 +3303,7 @@
   <dimension ref="A1:R1002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="O9" sqref="O9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3702,9 +3702,11 @@
         <v>63</v>
       </c>
       <c r="O9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="Q9" s="2" t="s">
         <v>65</v>
       </c>

</xml_diff>